<commit_message>
batch2 data cleaned and augmented
</commit_message>
<xml_diff>
--- a/notebooks/data/batch2_data/masquage patients batch2.xlsx
+++ b/notebooks/data/batch2_data/masquage patients batch2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louis/git/Tinnitus-n-Sleep/notebooks/data/batch2_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D14777-02C1-724C-B832-21912BDF7CE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B4F678-9613-3B40-88E9-E71FDFD4A107}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{B2F50F49-759A-41A5-90C9-0037ECFE677A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="68">
   <si>
     <t>1ZN04-soir-fin-juillet</t>
   </si>
@@ -72,9 +72,6 @@
     <t>060e9b4d-e761-11ea-be9b-2b562de1e2c7</t>
   </si>
   <si>
-    <t>1HS31</t>
-  </si>
-  <si>
     <t>789110bc-e765-11ea-be9b-2b562de1e2c7</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t>b565c2e1-e827-11ea-be9b-2b562de1e2c7</t>
   </si>
   <si>
-    <t>3SB04</t>
-  </si>
-  <si>
     <t>d0844a9d-e827-11ea-be9b-2b562de1e2c7</t>
   </si>
   <si>
@@ -220,13 +214,28 @@
   </si>
   <si>
     <t>Masking</t>
+  </si>
+  <si>
+    <t>3BS04</t>
+  </si>
+  <si>
+    <t>VAS_L_before</t>
+  </si>
+  <si>
+    <t>VAS_I_before</t>
+  </si>
+  <si>
+    <t>VAS_L_after</t>
+  </si>
+  <si>
+    <t>VAS_I_after</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,13 +243,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -252,17 +273,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -575,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C71369-88C2-4C60-B909-3010DBBDD714}">
-  <dimension ref="A1:P35"/>
+  <dimension ref="A1:T56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="S2" sqref="S2:T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -586,51 +610,63 @@
     <col min="11" max="11" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>52</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>53</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>54</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>55</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>56</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>57</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>58</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>59</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O1" t="s">
         <v>60</v>
       </c>
-      <c r="K1" t="s">
+      <c r="P1" t="s">
         <v>61</v>
       </c>
-      <c r="L1" t="s">
+      <c r="Q1" t="s">
         <v>64</v>
       </c>
-      <c r="O1" t="s">
-        <v>62</v>
-      </c>
-      <c r="P1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="R1" t="s">
+        <v>65</v>
+      </c>
+      <c r="S1" t="s">
+        <v>66</v>
+      </c>
+      <c r="T1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -680,8 +716,20 @@
         <f>L3</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q2" s="5">
+        <v>2</v>
+      </c>
+      <c r="R2" s="5">
+        <v>1</v>
+      </c>
+      <c r="S2" s="5">
+        <v>2</v>
+      </c>
+      <c r="T2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -721,7 +769,7 @@
       </c>
       <c r="N3" t="str">
         <f>A5</f>
-        <v>1HS31</v>
+        <v>1HS25</v>
       </c>
       <c r="O3">
         <f>L4</f>
@@ -731,8 +779,20 @@
         <f>L5</f>
         <v>12.666666666666666</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q3" s="5">
+        <v>2</v>
+      </c>
+      <c r="R3" s="5">
+        <v>2</v>
+      </c>
+      <c r="S3" s="5">
+        <v>6</v>
+      </c>
+      <c r="T3" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -782,10 +842,22 @@
         <f>L7</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q4" s="5">
+        <v>6</v>
+      </c>
+      <c r="R4" s="5">
+        <v>6</v>
+      </c>
+      <c r="S4" s="5">
+        <v>7</v>
+      </c>
+      <c r="T4" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
         <v>0.35416666666666669</v>
@@ -809,7 +881,7 @@
         <v>541</v>
       </c>
       <c r="I5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J5" s="2">
         <v>44069</v>
@@ -833,8 +905,20 @@
         <f>L9</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q5" s="5">
+        <v>4</v>
+      </c>
+      <c r="R5" s="5">
+        <v>5</v>
+      </c>
+      <c r="S5" s="5">
+        <v>3</v>
+      </c>
+      <c r="T5" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -884,8 +968,20 @@
         <f>L11</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q6" s="5">
+        <v>5</v>
+      </c>
+      <c r="R6" s="5">
+        <v>3</v>
+      </c>
+      <c r="S6" s="5">
+        <v>4</v>
+      </c>
+      <c r="T6" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -935,8 +1031,20 @@
         <f>L13</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q7" s="5">
+        <v>2</v>
+      </c>
+      <c r="R7" s="5">
+        <v>0</v>
+      </c>
+      <c r="S7" s="5">
+        <v>1</v>
+      </c>
+      <c r="T7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -986,8 +1094,20 @@
         <f>L15</f>
         <v>55.666666666666664</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q8" s="5">
+        <v>9</v>
+      </c>
+      <c r="R8" s="5">
+        <v>7</v>
+      </c>
+      <c r="S8" s="5">
+        <v>8</v>
+      </c>
+      <c r="T8" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1037,8 +1157,20 @@
         <f>L17</f>
         <v>6.333333333333333</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q9" s="5">
+        <v>4</v>
+      </c>
+      <c r="R9" s="5">
+        <v>2</v>
+      </c>
+      <c r="S9" s="5">
+        <v>3</v>
+      </c>
+      <c r="T9" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1078,7 +1210,7 @@
       </c>
       <c r="N10" t="str">
         <f>A19</f>
-        <v>3SB04</v>
+        <v>3BS04</v>
       </c>
       <c r="O10">
         <f>L18</f>
@@ -1088,8 +1220,20 @@
         <f>L19</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q10" s="5">
+        <v>6</v>
+      </c>
+      <c r="R10" s="5">
+        <v>6</v>
+      </c>
+      <c r="S10" s="5">
+        <v>5</v>
+      </c>
+      <c r="T10" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1139,10 +1283,22 @@
         <f>L21</f>
         <v>5.333333333333333</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q11" s="5">
+        <v>8</v>
+      </c>
+      <c r="R11" s="5">
+        <v>5</v>
+      </c>
+      <c r="S11" s="5">
+        <v>7</v>
+      </c>
+      <c r="T11" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1">
         <v>0.91180555555555554</v>
@@ -1166,7 +1322,7 @@
         <v>543</v>
       </c>
       <c r="I12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J12" s="2">
         <v>44069</v>
@@ -1190,10 +1346,22 @@
         <f>L23</f>
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q12" s="5">
+        <v>6</v>
+      </c>
+      <c r="R12" s="5">
+        <v>8</v>
+      </c>
+      <c r="S12" s="5">
+        <v>6</v>
+      </c>
+      <c r="T12" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1">
         <v>0.33333333333333331</v>
@@ -1217,7 +1385,7 @@
         <v>553</v>
       </c>
       <c r="I13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J13" s="2">
         <v>44070</v>
@@ -1241,10 +1409,22 @@
         <f>L25</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q13" s="5">
+        <v>2</v>
+      </c>
+      <c r="R13" s="5">
+        <v>1</v>
+      </c>
+      <c r="S13" s="5">
+        <v>4</v>
+      </c>
+      <c r="T13" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="1">
         <v>0.91319444444444453</v>
@@ -1268,7 +1448,7 @@
         <v>545</v>
       </c>
       <c r="I14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J14" s="2">
         <v>44070</v>
@@ -1292,10 +1472,22 @@
         <f>L27</f>
         <v>25.666666666666668</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q14" s="5">
+        <v>6</v>
+      </c>
+      <c r="R14" s="5">
+        <v>6</v>
+      </c>
+      <c r="S14" s="5">
+        <v>5</v>
+      </c>
+      <c r="T14" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1">
         <v>0.32847222222222222</v>
@@ -1319,7 +1511,7 @@
         <v>550</v>
       </c>
       <c r="I15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J15" s="2">
         <v>44070</v>
@@ -1343,10 +1535,22 @@
         <f>L29</f>
         <v>2.3333333333333335</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q15" s="5">
+        <v>3</v>
+      </c>
+      <c r="R15" s="5">
+        <v>2</v>
+      </c>
+      <c r="S15" s="5">
+        <v>2</v>
+      </c>
+      <c r="T15" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B16" s="1">
         <v>0.91875000000000007</v>
@@ -1370,7 +1574,7 @@
         <v>547</v>
       </c>
       <c r="I16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J16" s="2">
         <v>44070</v>
@@ -1394,10 +1598,22 @@
         <f>L31</f>
         <v>43.666666666666664</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q16" s="5">
+        <v>6</v>
+      </c>
+      <c r="R16" s="5">
+        <v>4</v>
+      </c>
+      <c r="S16" s="5">
+        <v>7</v>
+      </c>
+      <c r="T16" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B17" s="1">
         <v>0.34027777777777773</v>
@@ -1421,7 +1637,7 @@
         <v>549</v>
       </c>
       <c r="I17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J17" s="2">
         <v>44070</v>
@@ -1445,10 +1661,22 @@
         <f>L33</f>
         <v>2.6666666666666665</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q17" s="5">
+        <v>6</v>
+      </c>
+      <c r="R17" s="5">
+        <v>6</v>
+      </c>
+      <c r="S17" s="5">
+        <v>6</v>
+      </c>
+      <c r="T17" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="B18" s="1">
         <v>0.91666666666666663</v>
@@ -1472,7 +1700,7 @@
         <v>546</v>
       </c>
       <c r="I18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J18" s="2">
         <v>44070</v>
@@ -1485,9 +1713,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="B19" s="1">
         <v>0.33333333333333331</v>
@@ -1511,7 +1739,7 @@
         <v>551</v>
       </c>
       <c r="I19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J19" s="2">
         <v>44070</v>
@@ -1524,9 +1752,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B20" s="1">
         <v>0.875</v>
@@ -1550,7 +1778,7 @@
         <v>557</v>
       </c>
       <c r="I20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J20" s="2">
         <v>44071</v>
@@ -1563,9 +1791,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B21" s="1">
         <v>0.34097222222222223</v>
@@ -1589,7 +1817,7 @@
         <v>562</v>
       </c>
       <c r="I21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J21" s="2">
         <v>44071</v>
@@ -1602,9 +1830,9 @@
         <v>5.333333333333333</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B22" s="1">
         <v>0.87986111111111109</v>
@@ -1628,7 +1856,7 @@
         <v>558</v>
       </c>
       <c r="I22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J22" s="2">
         <v>44071</v>
@@ -1640,10 +1868,11 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T22" s="2"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B23" s="1">
         <v>0.30555555555555552</v>
@@ -1667,7 +1896,7 @@
         <v>560</v>
       </c>
       <c r="I23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J23" s="2">
         <v>44071</v>
@@ -1679,10 +1908,11 @@
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T23" s="2"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B24" s="1">
         <v>0.89374999999999993</v>
@@ -1706,7 +1936,7 @@
         <v>559</v>
       </c>
       <c r="I24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J24" s="2">
         <v>44071</v>
@@ -1719,9 +1949,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B25" s="1">
         <v>0.3444444444444445</v>
@@ -1745,7 +1975,7 @@
         <v>564</v>
       </c>
       <c r="I25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J25" s="2">
         <v>44071</v>
@@ -1757,10 +1987,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T25" s="2"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B26" s="1">
         <v>0.92083333333333339</v>
@@ -1784,7 +2015,7 @@
         <v>566</v>
       </c>
       <c r="I26" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J26" s="2">
         <v>44071</v>
@@ -1796,10 +2027,11 @@
         <f t="shared" si="0"/>
         <v>21.333333333333332</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T26" s="2"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B27" s="1">
         <v>0.32916666666666666</v>
@@ -1817,10 +2049,11 @@
         <f t="shared" si="0"/>
         <v>25.666666666666668</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T27" s="2"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B28" s="1">
         <v>0.86388888888888893</v>
@@ -1844,7 +2077,7 @@
         <v>567</v>
       </c>
       <c r="I28" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J28" s="2">
         <v>44071</v>
@@ -1856,10 +2089,11 @@
         <f t="shared" si="0"/>
         <v>2.6666666666666665</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T28" s="2"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B29" s="1">
         <v>0.32708333333333334</v>
@@ -1883,7 +2117,7 @@
         <v>573</v>
       </c>
       <c r="I29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J29" s="2">
         <v>44072</v>
@@ -1895,10 +2129,11 @@
         <f t="shared" si="0"/>
         <v>2.3333333333333335</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T29" s="2"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B30" s="1">
         <v>0.88750000000000007</v>
@@ -1922,7 +2157,7 @@
         <v>568</v>
       </c>
       <c r="I30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J30" s="2">
         <v>44071</v>
@@ -1934,10 +2169,11 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T30" s="2"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B31" s="1">
         <v>0.34861111111111115</v>
@@ -1961,7 +2197,7 @@
         <v>577</v>
       </c>
       <c r="I31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J31" s="2">
         <v>44072</v>
@@ -1973,10 +2209,11 @@
         <f t="shared" si="0"/>
         <v>43.666666666666664</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="T31" s="2"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B32" s="1">
         <v>0.94027777777777777</v>
@@ -2000,7 +2237,7 @@
         <v>571</v>
       </c>
       <c r="I32" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J32" s="2">
         <v>44072</v>
@@ -2012,10 +2249,11 @@
         <f t="shared" si="0"/>
         <v>3.6666666666666665</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="T32" s="2"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B33" s="1">
         <v>0.33958333333333335</v>
@@ -2039,7 +2277,7 @@
         <v>575</v>
       </c>
       <c r="I33" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J33" s="2">
         <v>44072</v>
@@ -2051,11 +2289,73 @@
         <f t="shared" si="0"/>
         <v>2.6666666666666665</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="T33" s="2"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T34" s="2"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
       <c r="J35" s="2"/>
       <c r="K35" s="3"/>
+      <c r="T35" s="2"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T36" s="2"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T37" s="2"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T38" s="2"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T39" s="2"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T40" s="2"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T41" s="2"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T42" s="2"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T43" s="2"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T44" s="2"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T45" s="2"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T46" s="2"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T47" s="2"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T48" s="2"/>
+    </row>
+    <row r="49" spans="20:20" x14ac:dyDescent="0.2">
+      <c r="T49" s="2"/>
+    </row>
+    <row r="51" spans="20:20" x14ac:dyDescent="0.2">
+      <c r="T51" s="2"/>
+    </row>
+    <row r="52" spans="20:20" x14ac:dyDescent="0.2">
+      <c r="T52" s="2"/>
+    </row>
+    <row r="53" spans="20:20" x14ac:dyDescent="0.2">
+      <c r="T53" s="2"/>
+    </row>
+    <row r="54" spans="20:20" x14ac:dyDescent="0.2">
+      <c r="T54" s="2"/>
+    </row>
+    <row r="56" spans="20:20" x14ac:dyDescent="0.2">
+      <c r="T56" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>